<commit_message>
datos de conducto propietario y vehiculo en pdf
</commit_message>
<xml_diff>
--- a/public/assets/templates/camioneta.xlsx
+++ b/public/assets/templates/camioneta.xlsx
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="132">
   <si>
     <t xml:space="preserve">INSPECCION MECANICA VEHICULAR PREVENTIVA</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">Vigencia Hasta:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATOS DEL PROPIETARIO</t>
   </si>
   <si>
     <t xml:space="preserve">Propietario</t>
@@ -600,7 +603,7 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFBFBFBF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -608,7 +611,7 @@
     <font>
       <b val="true"/>
       <sz val="16"/>
-      <color rgb="FFBFBFBF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1060,6 +1063,10 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
@@ -1068,17 +1075,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="11" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
@@ -1120,7 +1119,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1132,7 +1135,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1140,7 +1143,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1216,27 +1219,27 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1344,19 +1347,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1380,11 +1383,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1472,23 +1475,23 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1496,7 +1499,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1512,11 +1515,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1568,7 +1571,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1644,7 +1647,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1696,7 +1699,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1850,9 +1853,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2497680</xdr:colOff>
+      <xdr:colOff>2497320</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>237600</xdr:rowOff>
+      <xdr:rowOff>237240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1866,7 +1869,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="681840" y="555480"/>
-          <a:ext cx="2415960" cy="456120"/>
+          <a:ext cx="2415600" cy="455760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1888,8 +1891,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA48" activeCellId="0" sqref="W38:AA48"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10:AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2150,7 +2153,7 @@
       <c r="A10" s="6"/>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="25" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="25"/>
@@ -2162,42 +2165,42 @@
       <c r="K10" s="25"/>
       <c r="L10" s="25"/>
       <c r="M10" s="25"/>
-      <c r="N10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="O10" s="24"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="26"/>
-      <c r="S10" s="26"/>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-      <c r="V10" s="26"/>
-      <c r="W10" s="26"/>
-      <c r="X10" s="26"/>
-      <c r="Y10" s="26"/>
-      <c r="Z10" s="26"/>
-      <c r="AA10" s="26"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="25"/>
+      <c r="P10" s="25"/>
+      <c r="Q10" s="25"/>
+      <c r="R10" s="25"/>
+      <c r="S10" s="25"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
+      <c r="X10" s="25"/>
+      <c r="Y10" s="25"/>
+      <c r="Z10" s="25"/>
+      <c r="AA10" s="25"/>
       <c r="AB10" s="13"/>
     </row>
     <row r="11" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
+      <c r="K11" s="26"/>
+      <c r="L11" s="26"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="27"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="27"/>
-      <c r="K11" s="27"/>
-      <c r="L11" s="27"/>
-      <c r="M11" s="27"/>
-      <c r="N11" s="27"/>
-      <c r="O11" s="27"/>
+      <c r="O11" s="0"/>
       <c r="P11" s="27"/>
       <c r="Q11" s="27"/>
       <c r="R11" s="27"/>
@@ -2216,31 +2219,33 @@
       <c r="A12" s="6"/>
       <c r="B12" s="28"/>
       <c r="C12" s="8"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
-      <c r="I12" s="29"/>
-      <c r="J12" s="29"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="29"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="29"/>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-      <c r="T12" s="29"/>
-      <c r="U12" s="29"/>
-      <c r="V12" s="29"/>
-      <c r="W12" s="29"/>
-      <c r="X12" s="29"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="30"/>
+      <c r="D12" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="25"/>
+      <c r="Y12" s="25"/>
+      <c r="Z12" s="25"/>
+      <c r="AA12" s="25"/>
+      <c r="AB12" s="29"/>
       <c r="AC12" s="1"/>
       <c r="AD12" s="1"/>
       <c r="AE12" s="1"/>
@@ -2252,167 +2257,167 @@
       <c r="A13" s="6"/>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
-      <c r="D13" s="31" t="s">
-        <v>8</v>
+      <c r="D13" s="30" t="s">
+        <v>9</v>
       </c>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="32"/>
-      <c r="Q13" s="32"/>
-      <c r="R13" s="32"/>
-      <c r="S13" s="32"/>
-      <c r="T13" s="32"/>
-      <c r="U13" s="32"/>
-      <c r="V13" s="32"/>
-      <c r="W13" s="32"/>
-      <c r="X13" s="32"/>
-      <c r="Y13" s="32"/>
-      <c r="Z13" s="32"/>
-      <c r="AA13" s="32"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="31"/>
+      <c r="Q13" s="31"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="31"/>
+      <c r="T13" s="31"/>
+      <c r="U13" s="31"/>
+      <c r="V13" s="31"/>
+      <c r="W13" s="31"/>
+      <c r="X13" s="31"/>
+      <c r="Y13" s="31"/>
+      <c r="Z13" s="31"/>
+      <c r="AA13" s="31"/>
       <c r="AB13" s="13"/>
     </row>
     <row r="14" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="6"/>
       <c r="B14" s="7"/>
       <c r="C14" s="8"/>
-      <c r="D14" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="32"/>
-      <c r="H14" s="32"/>
-      <c r="I14" s="32"/>
-      <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="33" t="s">
+      <c r="D14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="O14" s="33"/>
-      <c r="P14" s="33"/>
-      <c r="Q14" s="33"/>
-      <c r="R14" s="33"/>
-      <c r="S14" s="33"/>
-      <c r="T14" s="33"/>
-      <c r="U14" s="32"/>
-      <c r="V14" s="32"/>
-      <c r="W14" s="32"/>
-      <c r="X14" s="32"/>
-      <c r="Y14" s="32"/>
-      <c r="Z14" s="32"/>
-      <c r="AA14" s="32"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="31"/>
+      <c r="H14" s="31"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="31"/>
+      <c r="L14" s="31"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="32"/>
+      <c r="R14" s="32"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="31"/>
+      <c r="V14" s="31"/>
+      <c r="W14" s="31"/>
+      <c r="X14" s="31"/>
+      <c r="Y14" s="31"/>
+      <c r="Z14" s="31"/>
+      <c r="AA14" s="31"/>
       <c r="AB14" s="13"/>
-      <c r="AE14" s="34"/>
-      <c r="AF14" s="34"/>
-      <c r="AG14" s="34"/>
-      <c r="AH14" s="34"/>
+      <c r="AE14" s="33"/>
+      <c r="AF14" s="33"/>
+      <c r="AG14" s="33"/>
+      <c r="AH14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
-      <c r="D15" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="E15" s="36"/>
-      <c r="F15" s="36"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="36"/>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
-      <c r="K15" s="36"/>
-      <c r="L15" s="36"/>
-      <c r="M15" s="36"/>
-      <c r="N15" s="37" t="s">
+      <c r="D15" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="O15" s="37"/>
-      <c r="P15" s="37"/>
-      <c r="Q15" s="37"/>
-      <c r="R15" s="37"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="38"/>
-      <c r="V15" s="38"/>
-      <c r="W15" s="38"/>
-      <c r="X15" s="38"/>
-      <c r="Y15" s="38"/>
-      <c r="Z15" s="38"/>
-      <c r="AA15" s="38"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="35"/>
+      <c r="H15" s="35"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
+      <c r="M15" s="35"/>
+      <c r="N15" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="O15" s="36"/>
+      <c r="P15" s="36"/>
+      <c r="Q15" s="36"/>
+      <c r="R15" s="36"/>
+      <c r="S15" s="36"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="37"/>
+      <c r="Z15" s="37"/>
+      <c r="AA15" s="37"/>
       <c r="AB15" s="13"/>
-      <c r="AE15" s="34"/>
-      <c r="AF15" s="34"/>
-      <c r="AG15" s="34"/>
-      <c r="AH15" s="34"/>
+      <c r="AE15" s="33"/>
+      <c r="AF15" s="33"/>
+      <c r="AG15" s="33"/>
+      <c r="AH15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
       <c r="B16" s="7"/>
       <c r="C16" s="8"/>
-      <c r="D16" s="39"/>
-      <c r="E16" s="39"/>
-      <c r="F16" s="39"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="40"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="39"/>
+      <c r="J16" s="39"/>
+      <c r="K16" s="39"/>
       <c r="L16" s="22"/>
       <c r="M16" s="23"/>
-      <c r="N16" s="40"/>
-      <c r="O16" s="40"/>
-      <c r="P16" s="40"/>
-      <c r="Q16" s="40"/>
-      <c r="R16" s="40"/>
-      <c r="S16" s="40"/>
-      <c r="T16" s="40"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="40"/>
+      <c r="N16" s="39"/>
+      <c r="O16" s="39"/>
+      <c r="P16" s="39"/>
+      <c r="Q16" s="39"/>
+      <c r="R16" s="39"/>
+      <c r="S16" s="39"/>
+      <c r="T16" s="39"/>
+      <c r="U16" s="39"/>
+      <c r="V16" s="39"/>
       <c r="W16" s="22"/>
       <c r="X16" s="22"/>
       <c r="Y16" s="22"/>
       <c r="Z16" s="22"/>
       <c r="AA16" s="22"/>
       <c r="AB16" s="13"/>
-      <c r="AE16" s="34"/>
-      <c r="AF16" s="34"/>
-      <c r="AG16" s="34"/>
-      <c r="AH16" s="34"/>
+      <c r="AE16" s="33"/>
+      <c r="AF16" s="33"/>
+      <c r="AG16" s="33"/>
+      <c r="AH16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="5.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
       <c r="B17" s="7"/>
       <c r="C17" s="8"/>
-      <c r="D17" s="39"/>
-      <c r="E17" s="39"/>
-      <c r="F17" s="39"/>
-      <c r="G17" s="39"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="40"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
       <c r="L17" s="22"/>
       <c r="M17" s="23"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
-      <c r="P17" s="40"/>
-      <c r="Q17" s="40"/>
-      <c r="R17" s="40"/>
-      <c r="S17" s="40"/>
-      <c r="T17" s="40"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="39"/>
+      <c r="P17" s="39"/>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="39"/>
+      <c r="S17" s="39"/>
+      <c r="T17" s="39"/>
+      <c r="U17" s="39"/>
+      <c r="V17" s="39"/>
       <c r="W17" s="22"/>
       <c r="X17" s="22"/>
       <c r="Y17" s="22"/>
@@ -2424,63 +2429,63 @@
       <c r="A18" s="6"/>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
-      <c r="D18" s="27" t="s">
-        <v>13</v>
+      <c r="D18" s="25" t="s">
+        <v>14</v>
       </c>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="27"/>
-      <c r="L18" s="27"/>
-      <c r="M18" s="27"/>
-      <c r="N18" s="27"/>
-      <c r="O18" s="27"/>
-      <c r="P18" s="27"/>
-      <c r="Q18" s="27"/>
-      <c r="R18" s="27"/>
-      <c r="S18" s="27"/>
-      <c r="T18" s="27"/>
-      <c r="U18" s="27"/>
-      <c r="V18" s="27"/>
-      <c r="W18" s="27"/>
-      <c r="X18" s="27"/>
-      <c r="Y18" s="27"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="27"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="25"/>
+      <c r="AA18" s="25"/>
       <c r="AB18" s="13"/>
     </row>
     <row r="19" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
       <c r="B19" s="28"/>
       <c r="C19" s="8"/>
-      <c r="D19" s="29"/>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="29"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="29"/>
-      <c r="Q19" s="29"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-      <c r="AA19" s="29"/>
-      <c r="AB19" s="30"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="40"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="40"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="40"/>
+      <c r="N19" s="40"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="40"/>
+      <c r="Q19" s="40"/>
+      <c r="R19" s="40"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="40"/>
+      <c r="U19" s="40"/>
+      <c r="V19" s="40"/>
+      <c r="W19" s="40"/>
+      <c r="X19" s="40"/>
+      <c r="Y19" s="40"/>
+      <c r="Z19" s="40"/>
+      <c r="AA19" s="40"/>
+      <c r="AB19" s="29"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
       <c r="AE19" s="1"/>
@@ -2493,7 +2498,7 @@
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
       <c r="D20" s="41" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
@@ -2504,22 +2509,22 @@
       <c r="K20" s="42"/>
       <c r="L20" s="42"/>
       <c r="M20" s="42"/>
-      <c r="N20" s="31" t="s">
-        <v>15</v>
+      <c r="N20" s="30" t="s">
+        <v>16</v>
       </c>
-      <c r="O20" s="31"/>
-      <c r="P20" s="31"/>
-      <c r="Q20" s="31"/>
-      <c r="R20" s="31"/>
-      <c r="S20" s="31"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="32"/>
-      <c r="W20" s="32"/>
-      <c r="X20" s="32"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="32"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="30"/>
+      <c r="T20" s="30"/>
+      <c r="U20" s="30"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="31"/>
+      <c r="X20" s="31"/>
+      <c r="Y20" s="31"/>
+      <c r="Z20" s="31"/>
+      <c r="AA20" s="31"/>
       <c r="AB20" s="13"/>
     </row>
     <row r="21" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2527,7 +2532,7 @@
       <c r="B21" s="7"/>
       <c r="C21" s="8"/>
       <c r="D21" s="41" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
@@ -2538,22 +2543,22 @@
       <c r="K21" s="42"/>
       <c r="L21" s="42"/>
       <c r="M21" s="42"/>
-      <c r="N21" s="31" t="s">
-        <v>17</v>
+      <c r="N21" s="30" t="s">
+        <v>18</v>
       </c>
-      <c r="O21" s="31"/>
-      <c r="P21" s="31"/>
-      <c r="Q21" s="31"/>
-      <c r="R21" s="31"/>
-      <c r="S21" s="31"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="32"/>
-      <c r="W21" s="32"/>
-      <c r="X21" s="32"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="32"/>
+      <c r="O21" s="30"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="30"/>
+      <c r="S21" s="30"/>
+      <c r="T21" s="30"/>
+      <c r="U21" s="30"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
       <c r="AB21" s="13"/>
     </row>
     <row r="22" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2561,7 +2566,7 @@
       <c r="B22" s="7"/>
       <c r="C22" s="8"/>
       <c r="D22" s="41" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E22" s="42"/>
       <c r="F22" s="42"/>
@@ -2572,22 +2577,22 @@
       <c r="K22" s="42"/>
       <c r="L22" s="42"/>
       <c r="M22" s="42"/>
-      <c r="N22" s="35" t="s">
-        <v>19</v>
+      <c r="N22" s="34" t="s">
+        <v>20</v>
       </c>
-      <c r="O22" s="35"/>
-      <c r="P22" s="35"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="35"/>
-      <c r="S22" s="35"/>
-      <c r="T22" s="35"/>
-      <c r="U22" s="35"/>
-      <c r="V22" s="36"/>
-      <c r="W22" s="36"/>
-      <c r="X22" s="36"/>
-      <c r="Y22" s="36"/>
-      <c r="Z22" s="36"/>
-      <c r="AA22" s="36"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
+      <c r="S22" s="34"/>
+      <c r="T22" s="34"/>
+      <c r="U22" s="34"/>
+      <c r="V22" s="35"/>
+      <c r="W22" s="35"/>
+      <c r="X22" s="35"/>
+      <c r="Y22" s="35"/>
+      <c r="Z22" s="35"/>
+      <c r="AA22" s="35"/>
       <c r="AB22" s="13"/>
     </row>
     <row r="23" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2595,35 +2600,35 @@
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
       <c r="D23" s="43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E23" s="44"/>
       <c r="F23" s="44"/>
       <c r="G23" s="44"/>
       <c r="H23" s="44"/>
       <c r="I23" s="45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J23" s="46"/>
       <c r="K23" s="46"/>
       <c r="L23" s="46"/>
       <c r="M23" s="46"/>
-      <c r="N23" s="35" t="s">
-        <v>22</v>
+      <c r="N23" s="34" t="s">
+        <v>23</v>
       </c>
-      <c r="O23" s="35"/>
-      <c r="P23" s="35"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
-      <c r="V23" s="32"/>
-      <c r="W23" s="32"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="32"/>
-      <c r="AA23" s="32"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="34"/>
+      <c r="T23" s="34"/>
+      <c r="U23" s="34"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="31"/>
       <c r="AB23" s="13"/>
     </row>
     <row r="24" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2631,35 +2636,35 @@
       <c r="B24" s="7"/>
       <c r="C24" s="8"/>
       <c r="D24" s="47" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E24" s="48"/>
       <c r="F24" s="48"/>
       <c r="G24" s="48"/>
       <c r="H24" s="48"/>
       <c r="I24" s="45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J24" s="46"/>
       <c r="K24" s="46"/>
       <c r="L24" s="46"/>
       <c r="M24" s="46"/>
-      <c r="N24" s="35" t="s">
-        <v>24</v>
+      <c r="N24" s="34" t="s">
+        <v>25</v>
       </c>
-      <c r="O24" s="35"/>
-      <c r="P24" s="35"/>
-      <c r="Q24" s="35"/>
-      <c r="R24" s="35"/>
-      <c r="S24" s="35"/>
-      <c r="T24" s="35"/>
-      <c r="U24" s="35"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
+      <c r="O24" s="34"/>
+      <c r="P24" s="34"/>
+      <c r="Q24" s="34"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
+      <c r="U24" s="34"/>
+      <c r="V24" s="35"/>
+      <c r="W24" s="35"/>
+      <c r="X24" s="35"/>
+      <c r="Y24" s="35"/>
+      <c r="Z24" s="35"/>
+      <c r="AA24" s="35"/>
       <c r="AB24" s="13"/>
     </row>
     <row r="25" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2667,35 +2672,35 @@
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
       <c r="D25" s="49" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E25" s="50"/>
       <c r="F25" s="50"/>
       <c r="G25" s="50"/>
       <c r="H25" s="50"/>
       <c r="I25" s="45" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J25" s="46"/>
       <c r="K25" s="46"/>
       <c r="L25" s="46"/>
       <c r="M25" s="46"/>
-      <c r="N25" s="35" t="s">
-        <v>26</v>
+      <c r="N25" s="34" t="s">
+        <v>27</v>
       </c>
-      <c r="O25" s="35"/>
-      <c r="P25" s="35"/>
-      <c r="Q25" s="35"/>
-      <c r="R25" s="35"/>
-      <c r="S25" s="35"/>
-      <c r="T25" s="35"/>
-      <c r="U25" s="35"/>
-      <c r="V25" s="36"/>
-      <c r="W25" s="36"/>
-      <c r="X25" s="36"/>
-      <c r="Y25" s="36"/>
-      <c r="Z25" s="36"/>
-      <c r="AA25" s="36"/>
+      <c r="O25" s="34"/>
+      <c r="P25" s="34"/>
+      <c r="Q25" s="34"/>
+      <c r="R25" s="34"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+      <c r="U25" s="34"/>
+      <c r="V25" s="35"/>
+      <c r="W25" s="35"/>
+      <c r="X25" s="35"/>
+      <c r="Y25" s="35"/>
+      <c r="Z25" s="35"/>
+      <c r="AA25" s="35"/>
       <c r="AB25" s="13"/>
     </row>
     <row r="26" customFormat="false" ht="9.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2732,63 +2737,63 @@
       <c r="A27" s="6"/>
       <c r="B27" s="7"/>
       <c r="C27" s="8"/>
-      <c r="D27" s="27" t="s">
-        <v>27</v>
+      <c r="D27" s="25" t="s">
+        <v>28</v>
       </c>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="27"/>
-      <c r="AA27" s="27"/>
+      <c r="E27" s="25"/>
+      <c r="F27" s="25"/>
+      <c r="G27" s="25"/>
+      <c r="H27" s="25"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="25"/>
+      <c r="R27" s="25"/>
+      <c r="S27" s="25"/>
+      <c r="T27" s="25"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="25"/>
+      <c r="W27" s="25"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
+      <c r="AA27" s="25"/>
       <c r="AB27" s="13"/>
     </row>
     <row r="28" customFormat="false" ht="6.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="6"/>
       <c r="B28" s="28"/>
       <c r="C28" s="8"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-      <c r="N28" s="29"/>
-      <c r="O28" s="29"/>
-      <c r="P28" s="29"/>
-      <c r="Q28" s="29"/>
-      <c r="R28" s="29"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="29"/>
-      <c r="U28" s="29"/>
-      <c r="V28" s="29"/>
-      <c r="W28" s="29"/>
-      <c r="X28" s="29"/>
-      <c r="Y28" s="29"/>
-      <c r="Z28" s="29"/>
-      <c r="AA28" s="29"/>
-      <c r="AB28" s="30"/>
+      <c r="D28" s="40"/>
+      <c r="E28" s="40"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="40"/>
+      <c r="N28" s="40"/>
+      <c r="O28" s="40"/>
+      <c r="P28" s="40"/>
+      <c r="Q28" s="40"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="40"/>
+      <c r="T28" s="40"/>
+      <c r="U28" s="40"/>
+      <c r="V28" s="40"/>
+      <c r="W28" s="40"/>
+      <c r="X28" s="40"/>
+      <c r="Y28" s="40"/>
+      <c r="Z28" s="40"/>
+      <c r="AA28" s="40"/>
+      <c r="AB28" s="29"/>
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
@@ -2801,7 +2806,7 @@
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
       <c r="D29" s="52" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E29" s="52"/>
       <c r="F29" s="52"/>
@@ -2893,7 +2898,7 @@
       <c r="B32" s="7"/>
       <c r="C32" s="8"/>
       <c r="D32" s="54" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E32" s="55"/>
       <c r="F32" s="53"/>
@@ -2910,7 +2915,7 @@
       <c r="Q32" s="53"/>
       <c r="R32" s="53"/>
       <c r="S32" s="53" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T32" s="53"/>
       <c r="U32" s="53"/>
@@ -2927,21 +2932,21 @@
       <c r="B33" s="7"/>
       <c r="C33" s="8"/>
       <c r="D33" s="56" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E33" s="57"/>
       <c r="F33" s="23"/>
       <c r="G33" s="58" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
-      <c r="H33" s="34"/>
+      <c r="H33" s="33"/>
       <c r="I33" s="59"/>
       <c r="J33" s="59"/>
       <c r="K33" s="59"/>
       <c r="L33" s="60"/>
       <c r="M33" s="61"/>
       <c r="N33" s="61" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O33" s="62"/>
       <c r="P33" s="61"/>
@@ -2999,7 +3004,7 @@
       <c r="B35" s="7"/>
       <c r="C35" s="8"/>
       <c r="D35" s="63" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E35" s="63"/>
       <c r="F35" s="63"/>
@@ -3010,22 +3015,22 @@
       <c r="K35" s="63"/>
       <c r="L35" s="63"/>
       <c r="M35" s="64"/>
-      <c r="N35" s="27" t="s">
-        <v>35</v>
+      <c r="N35" s="25" t="s">
+        <v>36</v>
       </c>
-      <c r="O35" s="27"/>
-      <c r="P35" s="27"/>
-      <c r="Q35" s="27"/>
-      <c r="R35" s="27"/>
-      <c r="S35" s="27"/>
-      <c r="T35" s="27"/>
-      <c r="U35" s="27"/>
-      <c r="V35" s="27"/>
-      <c r="W35" s="27"/>
-      <c r="X35" s="27"/>
-      <c r="Y35" s="27"/>
-      <c r="Z35" s="27"/>
-      <c r="AA35" s="27"/>
+      <c r="O35" s="25"/>
+      <c r="P35" s="25"/>
+      <c r="Q35" s="25"/>
+      <c r="R35" s="25"/>
+      <c r="S35" s="25"/>
+      <c r="T35" s="25"/>
+      <c r="U35" s="25"/>
+      <c r="V35" s="25"/>
+      <c r="W35" s="25"/>
+      <c r="X35" s="25"/>
+      <c r="Y35" s="25"/>
+      <c r="Z35" s="25"/>
+      <c r="AA35" s="25"/>
       <c r="AB35" s="13"/>
     </row>
     <row r="36" customFormat="false" ht="6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3042,20 +3047,20 @@
       <c r="K36" s="64"/>
       <c r="L36" s="64"/>
       <c r="M36" s="64"/>
-      <c r="N36" s="29"/>
-      <c r="O36" s="29"/>
-      <c r="P36" s="29"/>
-      <c r="Q36" s="29"/>
-      <c r="R36" s="29"/>
-      <c r="S36" s="29"/>
-      <c r="T36" s="29"/>
-      <c r="U36" s="29"/>
-      <c r="V36" s="29"/>
-      <c r="W36" s="29"/>
-      <c r="X36" s="29"/>
-      <c r="Y36" s="29"/>
-      <c r="Z36" s="29"/>
-      <c r="AA36" s="29"/>
+      <c r="N36" s="40"/>
+      <c r="O36" s="40"/>
+      <c r="P36" s="40"/>
+      <c r="Q36" s="40"/>
+      <c r="R36" s="40"/>
+      <c r="S36" s="40"/>
+      <c r="T36" s="40"/>
+      <c r="U36" s="40"/>
+      <c r="V36" s="40"/>
+      <c r="W36" s="40"/>
+      <c r="X36" s="40"/>
+      <c r="Y36" s="40"/>
+      <c r="Z36" s="40"/>
+      <c r="AA36" s="40"/>
       <c r="AB36" s="13"/>
       <c r="AC36" s="1"/>
       <c r="AD36" s="1"/>
@@ -3069,25 +3074,25 @@
       <c r="B37" s="7"/>
       <c r="C37" s="8"/>
       <c r="D37" s="65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E37" s="65"/>
       <c r="F37" s="66"/>
       <c r="G37" s="66"/>
       <c r="H37" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I37" s="67"/>
       <c r="J37" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K37" s="67"/>
       <c r="L37" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
-      <c r="M37" s="29"/>
+      <c r="M37" s="40"/>
       <c r="N37" s="68" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O37" s="68"/>
       <c r="P37" s="68"/>
@@ -3098,15 +3103,15 @@
       <c r="U37" s="69"/>
       <c r="V37" s="69"/>
       <c r="W37" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X37" s="67"/>
       <c r="Y37" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z37" s="67"/>
       <c r="AA37" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB37" s="13"/>
     </row>
@@ -3115,13 +3120,13 @@
       <c r="B38" s="7"/>
       <c r="C38" s="8"/>
       <c r="D38" s="70" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E38" s="70"/>
       <c r="F38" s="70"/>
       <c r="G38" s="70"/>
       <c r="H38" s="71" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="I38" s="72"/>
       <c r="J38" s="73"/>
@@ -3129,7 +3134,7 @@
       <c r="L38" s="74"/>
       <c r="M38" s="75"/>
       <c r="N38" s="76" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O38" s="76"/>
       <c r="P38" s="76"/>
@@ -3192,7 +3197,7 @@
       <c r="B40" s="7"/>
       <c r="C40" s="8"/>
       <c r="D40" s="84" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E40" s="84"/>
       <c r="F40" s="84"/>
@@ -3204,7 +3209,7 @@
       <c r="L40" s="74"/>
       <c r="M40" s="75"/>
       <c r="N40" s="85" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="O40" s="85"/>
       <c r="P40" s="85"/>
@@ -3268,7 +3273,7 @@
       <c r="B42" s="7"/>
       <c r="C42" s="8"/>
       <c r="D42" s="88" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E42" s="88"/>
       <c r="F42" s="88"/>
@@ -3280,7 +3285,7 @@
       <c r="L42" s="74"/>
       <c r="M42" s="75"/>
       <c r="N42" s="76" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="O42" s="76"/>
       <c r="P42" s="76"/>
@@ -3344,7 +3349,7 @@
       <c r="B44" s="7"/>
       <c r="C44" s="8"/>
       <c r="D44" s="89" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E44" s="89"/>
       <c r="F44" s="89"/>
@@ -3356,7 +3361,7 @@
       <c r="L44" s="74"/>
       <c r="M44" s="75"/>
       <c r="N44" s="85" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="O44" s="85"/>
       <c r="P44" s="85"/>
@@ -3420,7 +3425,7 @@
       <c r="B46" s="7"/>
       <c r="C46" s="8"/>
       <c r="D46" s="90" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E46" s="90"/>
       <c r="F46" s="90"/>
@@ -3432,7 +3437,7 @@
       <c r="L46" s="74"/>
       <c r="M46" s="75"/>
       <c r="N46" s="76" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O46" s="91"/>
       <c r="P46" s="76"/>
@@ -3496,7 +3501,7 @@
       <c r="B48" s="7"/>
       <c r="C48" s="8"/>
       <c r="D48" s="84" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E48" s="84"/>
       <c r="F48" s="84"/>
@@ -3508,7 +3513,7 @@
       <c r="L48" s="74"/>
       <c r="M48" s="75"/>
       <c r="N48" s="93" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O48" s="93"/>
       <c r="P48" s="93"/>
@@ -3572,7 +3577,7 @@
       <c r="B50" s="7"/>
       <c r="C50" s="8"/>
       <c r="D50" s="70" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E50" s="70"/>
       <c r="F50" s="70"/>
@@ -3584,7 +3589,7 @@
       <c r="L50" s="74"/>
       <c r="M50" s="75"/>
       <c r="N50" s="95" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="O50" s="95"/>
       <c r="P50" s="95"/>
@@ -3621,20 +3626,20 @@
       <c r="K51" s="72"/>
       <c r="L51" s="87"/>
       <c r="M51" s="75"/>
-      <c r="N51" s="29"/>
-      <c r="O51" s="29"/>
-      <c r="P51" s="29"/>
-      <c r="Q51" s="29"/>
-      <c r="R51" s="29"/>
-      <c r="S51" s="29"/>
-      <c r="T51" s="29"/>
-      <c r="U51" s="29"/>
-      <c r="V51" s="29"/>
-      <c r="W51" s="29"/>
-      <c r="X51" s="29"/>
-      <c r="Y51" s="29"/>
-      <c r="Z51" s="29"/>
-      <c r="AA51" s="29"/>
+      <c r="N51" s="40"/>
+      <c r="O51" s="40"/>
+      <c r="P51" s="40"/>
+      <c r="Q51" s="40"/>
+      <c r="R51" s="40"/>
+      <c r="S51" s="40"/>
+      <c r="T51" s="40"/>
+      <c r="U51" s="40"/>
+      <c r="V51" s="40"/>
+      <c r="W51" s="40"/>
+      <c r="X51" s="40"/>
+      <c r="Y51" s="40"/>
+      <c r="Z51" s="40"/>
+      <c r="AA51" s="40"/>
       <c r="AB51" s="96"/>
       <c r="AC51" s="1"/>
       <c r="AD51" s="1"/>
@@ -3648,7 +3653,7 @@
       <c r="B52" s="7"/>
       <c r="C52" s="8"/>
       <c r="D52" s="84" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E52" s="84"/>
       <c r="F52" s="84"/>
@@ -3660,7 +3665,7 @@
       <c r="L52" s="74"/>
       <c r="M52" s="75"/>
       <c r="N52" s="97" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O52" s="97"/>
       <c r="P52" s="97"/>
@@ -3671,15 +3676,15 @@
       <c r="U52" s="98"/>
       <c r="V52" s="98"/>
       <c r="W52" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X52" s="67"/>
       <c r="Y52" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z52" s="67"/>
       <c r="AA52" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB52" s="99"/>
       <c r="AC52" s="1"/>
@@ -3703,20 +3708,20 @@
       <c r="K53" s="72"/>
       <c r="L53" s="83"/>
       <c r="M53" s="75"/>
-      <c r="N53" s="29"/>
-      <c r="O53" s="29"/>
-      <c r="P53" s="29"/>
-      <c r="Q53" s="29"/>
-      <c r="R53" s="29"/>
-      <c r="S53" s="29"/>
-      <c r="T53" s="29"/>
-      <c r="U53" s="29"/>
-      <c r="V53" s="29"/>
-      <c r="W53" s="29"/>
-      <c r="X53" s="29"/>
-      <c r="Y53" s="29"/>
-      <c r="Z53" s="29"/>
-      <c r="AA53" s="29"/>
+      <c r="N53" s="40"/>
+      <c r="O53" s="40"/>
+      <c r="P53" s="40"/>
+      <c r="Q53" s="40"/>
+      <c r="R53" s="40"/>
+      <c r="S53" s="40"/>
+      <c r="T53" s="40"/>
+      <c r="U53" s="40"/>
+      <c r="V53" s="40"/>
+      <c r="W53" s="40"/>
+      <c r="X53" s="40"/>
+      <c r="Y53" s="40"/>
+      <c r="Z53" s="40"/>
+      <c r="AA53" s="40"/>
       <c r="AB53" s="96"/>
       <c r="AC53" s="1"/>
       <c r="AD53" s="1"/>
@@ -3730,7 +3735,7 @@
       <c r="B54" s="7"/>
       <c r="C54" s="8"/>
       <c r="D54" s="70" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E54" s="70"/>
       <c r="F54" s="70"/>
@@ -3742,7 +3747,7 @@
       <c r="L54" s="74"/>
       <c r="M54" s="75"/>
       <c r="N54" s="85" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="O54" s="85"/>
       <c r="P54" s="85"/>
@@ -3806,7 +3811,7 @@
       <c r="B56" s="7"/>
       <c r="C56" s="8"/>
       <c r="D56" s="84" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E56" s="84"/>
       <c r="F56" s="84"/>
@@ -3818,7 +3823,7 @@
       <c r="L56" s="74"/>
       <c r="M56" s="75"/>
       <c r="N56" s="76" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="O56" s="76"/>
       <c r="P56" s="76"/>
@@ -3882,7 +3887,7 @@
       <c r="B58" s="7"/>
       <c r="C58" s="8"/>
       <c r="D58" s="101" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E58" s="101"/>
       <c r="F58" s="101"/>
@@ -3894,7 +3899,7 @@
       <c r="L58" s="74"/>
       <c r="M58" s="75"/>
       <c r="N58" s="85" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="O58" s="85"/>
       <c r="P58" s="85"/>
@@ -3958,7 +3963,7 @@
       <c r="B60" s="7"/>
       <c r="C60" s="8"/>
       <c r="D60" s="84" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E60" s="84"/>
       <c r="F60" s="84"/>
@@ -3970,7 +3975,7 @@
       <c r="L60" s="74"/>
       <c r="M60" s="103"/>
       <c r="N60" s="76" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="O60" s="76"/>
       <c r="P60" s="76"/>
@@ -4034,7 +4039,7 @@
       <c r="B62" s="7"/>
       <c r="C62" s="8"/>
       <c r="D62" s="63" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E62" s="63"/>
       <c r="F62" s="63"/>
@@ -4046,7 +4051,7 @@
       <c r="L62" s="63"/>
       <c r="M62" s="64"/>
       <c r="N62" s="85" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="O62" s="85"/>
       <c r="P62" s="85"/>
@@ -4104,25 +4109,25 @@
       <c r="B64" s="7"/>
       <c r="C64" s="8"/>
       <c r="D64" s="65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E64" s="65"/>
       <c r="F64" s="66"/>
       <c r="G64" s="66"/>
       <c r="H64" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I64" s="67"/>
       <c r="J64" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K64" s="67"/>
       <c r="L64" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
-      <c r="M64" s="29"/>
+      <c r="M64" s="40"/>
       <c r="N64" s="76" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="O64" s="76"/>
       <c r="P64" s="76"/>
@@ -4143,16 +4148,16 @@
       <c r="A65" s="6"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8"/>
-      <c r="D65" s="29"/>
-      <c r="E65" s="29"/>
-      <c r="F65" s="29"/>
-      <c r="G65" s="29"/>
-      <c r="H65" s="29"/>
-      <c r="I65" s="29"/>
-      <c r="J65" s="29"/>
-      <c r="K65" s="29"/>
-      <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+      <c r="I65" s="40"/>
+      <c r="J65" s="40"/>
+      <c r="K65" s="40"/>
+      <c r="L65" s="40"/>
+      <c r="M65" s="40"/>
       <c r="N65" s="76"/>
       <c r="O65" s="76"/>
       <c r="P65" s="76"/>
@@ -4180,7 +4185,7 @@
       <c r="B66" s="7"/>
       <c r="C66" s="8"/>
       <c r="D66" s="90" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E66" s="90"/>
       <c r="F66" s="90"/>
@@ -4192,7 +4197,7 @@
       <c r="L66" s="79"/>
       <c r="M66" s="75"/>
       <c r="N66" s="93" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O66" s="93"/>
       <c r="P66" s="93"/>
@@ -4256,7 +4261,7 @@
       <c r="B68" s="7"/>
       <c r="C68" s="8"/>
       <c r="D68" s="104" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E68" s="104"/>
       <c r="F68" s="104"/>
@@ -4267,22 +4272,22 @@
       <c r="K68" s="72"/>
       <c r="L68" s="79"/>
       <c r="M68" s="75"/>
-      <c r="N68" s="27" t="s">
-        <v>70</v>
+      <c r="N68" s="25" t="s">
+        <v>71</v>
       </c>
-      <c r="O68" s="27"/>
-      <c r="P68" s="27"/>
-      <c r="Q68" s="27"/>
-      <c r="R68" s="27"/>
-      <c r="S68" s="27"/>
-      <c r="T68" s="27"/>
-      <c r="U68" s="27"/>
-      <c r="V68" s="27"/>
-      <c r="W68" s="27"/>
-      <c r="X68" s="27"/>
-      <c r="Y68" s="27"/>
-      <c r="Z68" s="27"/>
-      <c r="AA68" s="27"/>
+      <c r="O68" s="25"/>
+      <c r="P68" s="25"/>
+      <c r="Q68" s="25"/>
+      <c r="R68" s="25"/>
+      <c r="S68" s="25"/>
+      <c r="T68" s="25"/>
+      <c r="U68" s="25"/>
+      <c r="V68" s="25"/>
+      <c r="W68" s="25"/>
+      <c r="X68" s="25"/>
+      <c r="Y68" s="25"/>
+      <c r="Z68" s="25"/>
+      <c r="AA68" s="25"/>
       <c r="AB68" s="105"/>
       <c r="AC68" s="1"/>
       <c r="AD68" s="1"/>
@@ -4305,20 +4310,20 @@
       <c r="K69" s="72"/>
       <c r="L69" s="72"/>
       <c r="M69" s="75"/>
-      <c r="N69" s="29"/>
-      <c r="O69" s="29"/>
-      <c r="P69" s="29"/>
-      <c r="Q69" s="29"/>
-      <c r="R69" s="29"/>
-      <c r="S69" s="29"/>
-      <c r="T69" s="29"/>
-      <c r="U69" s="29"/>
-      <c r="V69" s="29"/>
-      <c r="W69" s="29"/>
-      <c r="X69" s="29"/>
-      <c r="Y69" s="29"/>
-      <c r="Z69" s="29"/>
-      <c r="AA69" s="29"/>
+      <c r="N69" s="40"/>
+      <c r="O69" s="40"/>
+      <c r="P69" s="40"/>
+      <c r="Q69" s="40"/>
+      <c r="R69" s="40"/>
+      <c r="S69" s="40"/>
+      <c r="T69" s="40"/>
+      <c r="U69" s="40"/>
+      <c r="V69" s="40"/>
+      <c r="W69" s="40"/>
+      <c r="X69" s="40"/>
+      <c r="Y69" s="40"/>
+      <c r="Z69" s="40"/>
+      <c r="AA69" s="40"/>
       <c r="AB69" s="96"/>
       <c r="AC69" s="1"/>
       <c r="AD69" s="1"/>
@@ -4332,7 +4337,7 @@
       <c r="B70" s="7"/>
       <c r="C70" s="8"/>
       <c r="D70" s="90" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E70" s="90"/>
       <c r="F70" s="90"/>
@@ -4344,26 +4349,26 @@
       <c r="L70" s="79"/>
       <c r="M70" s="75"/>
       <c r="N70" s="106" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O70" s="106"/>
       <c r="P70" s="106"/>
       <c r="Q70" s="106"/>
       <c r="R70" s="106"/>
       <c r="S70" s="106"/>
-      <c r="T70" s="29"/>
-      <c r="U70" s="29"/>
-      <c r="V70" s="29"/>
+      <c r="T70" s="40"/>
+      <c r="U70" s="40"/>
+      <c r="V70" s="40"/>
       <c r="W70" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X70" s="67"/>
       <c r="Y70" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z70" s="67"/>
       <c r="AA70" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB70" s="105"/>
       <c r="AC70" s="1"/>
@@ -4387,20 +4392,20 @@
       <c r="K71" s="72"/>
       <c r="L71" s="107"/>
       <c r="M71" s="75"/>
-      <c r="N71" s="29"/>
-      <c r="O71" s="29"/>
-      <c r="P71" s="29"/>
-      <c r="Q71" s="29"/>
-      <c r="R71" s="29"/>
-      <c r="S71" s="29"/>
-      <c r="T71" s="29"/>
-      <c r="U71" s="29"/>
-      <c r="V71" s="29"/>
-      <c r="W71" s="29"/>
-      <c r="X71" s="29"/>
-      <c r="Y71" s="29"/>
-      <c r="Z71" s="29"/>
-      <c r="AA71" s="29"/>
+      <c r="N71" s="40"/>
+      <c r="O71" s="40"/>
+      <c r="P71" s="40"/>
+      <c r="Q71" s="40"/>
+      <c r="R71" s="40"/>
+      <c r="S71" s="40"/>
+      <c r="T71" s="40"/>
+      <c r="U71" s="40"/>
+      <c r="V71" s="40"/>
+      <c r="W71" s="40"/>
+      <c r="X71" s="40"/>
+      <c r="Y71" s="40"/>
+      <c r="Z71" s="40"/>
+      <c r="AA71" s="40"/>
       <c r="AB71" s="96"/>
       <c r="AC71" s="1"/>
       <c r="AD71" s="1"/>
@@ -4414,7 +4419,7 @@
       <c r="B72" s="7"/>
       <c r="C72" s="8"/>
       <c r="D72" s="104" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E72" s="104"/>
       <c r="F72" s="104"/>
@@ -4426,7 +4431,7 @@
       <c r="L72" s="79"/>
       <c r="M72" s="75"/>
       <c r="N72" s="89" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="O72" s="89"/>
       <c r="P72" s="89"/>
@@ -4490,7 +4495,7 @@
       <c r="B74" s="7"/>
       <c r="C74" s="8"/>
       <c r="D74" s="90" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E74" s="90"/>
       <c r="F74" s="90"/>
@@ -4502,7 +4507,7 @@
       <c r="L74" s="79"/>
       <c r="M74" s="75"/>
       <c r="N74" s="88" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="O74" s="88"/>
       <c r="P74" s="88"/>
@@ -4566,7 +4571,7 @@
       <c r="B76" s="7"/>
       <c r="C76" s="8"/>
       <c r="D76" s="104" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E76" s="104"/>
       <c r="F76" s="104"/>
@@ -4578,7 +4583,7 @@
       <c r="L76" s="79"/>
       <c r="M76" s="75"/>
       <c r="N76" s="113" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="O76" s="113"/>
       <c r="P76" s="113"/>
@@ -4642,7 +4647,7 @@
       <c r="B78" s="7"/>
       <c r="C78" s="8"/>
       <c r="D78" s="90" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E78" s="90"/>
       <c r="F78" s="90"/>
@@ -4654,7 +4659,7 @@
       <c r="L78" s="79"/>
       <c r="M78" s="75"/>
       <c r="N78" s="76" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="O78" s="76"/>
       <c r="P78" s="76"/>
@@ -4717,20 +4722,20 @@
       <c r="A80" s="6"/>
       <c r="B80" s="7"/>
       <c r="C80" s="8"/>
-      <c r="D80" s="27" t="s">
-        <v>80</v>
+      <c r="D80" s="25" t="s">
+        <v>81</v>
       </c>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="27"/>
-      <c r="H80" s="27"/>
-      <c r="I80" s="27"/>
-      <c r="J80" s="27"/>
-      <c r="K80" s="27"/>
-      <c r="L80" s="27"/>
-      <c r="M80" s="29"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="25"/>
+      <c r="H80" s="25"/>
+      <c r="I80" s="25"/>
+      <c r="J80" s="25"/>
+      <c r="K80" s="25"/>
+      <c r="L80" s="25"/>
+      <c r="M80" s="40"/>
       <c r="N80" s="85" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="O80" s="85"/>
       <c r="P80" s="85"/>
@@ -4757,16 +4762,16 @@
       <c r="A81" s="6"/>
       <c r="B81" s="7"/>
       <c r="C81" s="8"/>
-      <c r="D81" s="29"/>
-      <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="29"/>
-      <c r="H81" s="29"/>
-      <c r="I81" s="29"/>
-      <c r="J81" s="29"/>
-      <c r="K81" s="29"/>
-      <c r="L81" s="29"/>
-      <c r="M81" s="29"/>
+      <c r="D81" s="40"/>
+      <c r="E81" s="40"/>
+      <c r="F81" s="40"/>
+      <c r="G81" s="40"/>
+      <c r="H81" s="40"/>
+      <c r="I81" s="40"/>
+      <c r="J81" s="40"/>
+      <c r="K81" s="40"/>
+      <c r="L81" s="40"/>
+      <c r="M81" s="40"/>
       <c r="N81" s="76"/>
       <c r="O81" s="76"/>
       <c r="P81" s="76"/>
@@ -4794,25 +4799,25 @@
       <c r="B82" s="7"/>
       <c r="C82" s="8"/>
       <c r="D82" s="65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E82" s="65"/>
       <c r="F82" s="66"/>
       <c r="G82" s="66"/>
       <c r="H82" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I82" s="67"/>
       <c r="J82" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K82" s="67"/>
       <c r="L82" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
-      <c r="M82" s="29"/>
+      <c r="M82" s="40"/>
       <c r="N82" s="88" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="O82" s="88"/>
       <c r="P82" s="88"/>
@@ -4833,16 +4838,16 @@
       <c r="A83" s="6"/>
       <c r="B83" s="7"/>
       <c r="C83" s="8"/>
-      <c r="D83" s="29"/>
-      <c r="E83" s="29"/>
-      <c r="F83" s="29"/>
-      <c r="G83" s="29"/>
-      <c r="H83" s="29"/>
-      <c r="I83" s="29"/>
-      <c r="J83" s="29"/>
-      <c r="K83" s="29"/>
-      <c r="L83" s="29"/>
-      <c r="M83" s="29"/>
+      <c r="D83" s="40"/>
+      <c r="E83" s="40"/>
+      <c r="F83" s="40"/>
+      <c r="G83" s="40"/>
+      <c r="H83" s="40"/>
+      <c r="I83" s="40"/>
+      <c r="J83" s="40"/>
+      <c r="K83" s="40"/>
+      <c r="L83" s="40"/>
+      <c r="M83" s="40"/>
       <c r="N83" s="53"/>
       <c r="O83" s="53"/>
       <c r="P83" s="53"/>
@@ -4870,7 +4875,7 @@
       <c r="B84" s="7"/>
       <c r="C84" s="8"/>
       <c r="D84" s="116" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E84" s="116"/>
       <c r="F84" s="116"/>
@@ -4882,7 +4887,7 @@
       <c r="L84" s="79"/>
       <c r="M84" s="75"/>
       <c r="N84" s="85" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="O84" s="85"/>
       <c r="P84" s="85"/>
@@ -4940,7 +4945,7 @@
       <c r="B86" s="7"/>
       <c r="C86" s="8"/>
       <c r="D86" s="119" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E86" s="119"/>
       <c r="F86" s="119"/>
@@ -4952,7 +4957,7 @@
       <c r="L86" s="79"/>
       <c r="M86" s="75"/>
       <c r="N86" s="88" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O86" s="88"/>
       <c r="P86" s="88"/>
@@ -5016,7 +5021,7 @@
       <c r="B88" s="7"/>
       <c r="C88" s="8"/>
       <c r="D88" s="116" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="E88" s="116"/>
       <c r="F88" s="116"/>
@@ -5027,22 +5032,22 @@
       <c r="K88" s="72"/>
       <c r="L88" s="79"/>
       <c r="M88" s="75"/>
-      <c r="N88" s="27" t="s">
-        <v>88</v>
+      <c r="N88" s="25" t="s">
+        <v>89</v>
       </c>
-      <c r="O88" s="27"/>
-      <c r="P88" s="27"/>
-      <c r="Q88" s="27"/>
-      <c r="R88" s="27"/>
-      <c r="S88" s="27"/>
-      <c r="T88" s="27"/>
-      <c r="U88" s="27"/>
-      <c r="V88" s="27"/>
-      <c r="W88" s="27"/>
-      <c r="X88" s="27"/>
-      <c r="Y88" s="27"/>
-      <c r="Z88" s="27"/>
-      <c r="AA88" s="27"/>
+      <c r="O88" s="25"/>
+      <c r="P88" s="25"/>
+      <c r="Q88" s="25"/>
+      <c r="R88" s="25"/>
+      <c r="S88" s="25"/>
+      <c r="T88" s="25"/>
+      <c r="U88" s="25"/>
+      <c r="V88" s="25"/>
+      <c r="W88" s="25"/>
+      <c r="X88" s="25"/>
+      <c r="Y88" s="25"/>
+      <c r="Z88" s="25"/>
+      <c r="AA88" s="25"/>
       <c r="AB88" s="105"/>
       <c r="AC88" s="1"/>
       <c r="AD88" s="1"/>
@@ -5065,20 +5070,20 @@
       <c r="K89" s="72"/>
       <c r="L89" s="72"/>
       <c r="M89" s="75"/>
-      <c r="N89" s="29"/>
-      <c r="O89" s="29"/>
-      <c r="P89" s="29"/>
-      <c r="Q89" s="29"/>
-      <c r="R89" s="29"/>
-      <c r="S89" s="29"/>
-      <c r="T89" s="29"/>
-      <c r="U89" s="29"/>
-      <c r="V89" s="29"/>
-      <c r="W89" s="29"/>
-      <c r="X89" s="29"/>
-      <c r="Y89" s="29"/>
-      <c r="Z89" s="29"/>
-      <c r="AA89" s="29"/>
+      <c r="N89" s="40"/>
+      <c r="O89" s="40"/>
+      <c r="P89" s="40"/>
+      <c r="Q89" s="40"/>
+      <c r="R89" s="40"/>
+      <c r="S89" s="40"/>
+      <c r="T89" s="40"/>
+      <c r="U89" s="40"/>
+      <c r="V89" s="40"/>
+      <c r="W89" s="40"/>
+      <c r="X89" s="40"/>
+      <c r="Y89" s="40"/>
+      <c r="Z89" s="40"/>
+      <c r="AA89" s="40"/>
       <c r="AB89" s="96"/>
       <c r="AC89" s="1"/>
       <c r="AD89" s="1"/>
@@ -5092,7 +5097,7 @@
       <c r="B90" s="7"/>
       <c r="C90" s="8"/>
       <c r="D90" s="119" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E90" s="119"/>
       <c r="F90" s="119"/>
@@ -5104,26 +5109,26 @@
       <c r="L90" s="79"/>
       <c r="M90" s="75"/>
       <c r="N90" s="106" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O90" s="106"/>
       <c r="P90" s="106"/>
       <c r="Q90" s="106"/>
       <c r="R90" s="106"/>
       <c r="S90" s="106"/>
-      <c r="T90" s="29"/>
-      <c r="U90" s="29"/>
-      <c r="V90" s="29"/>
+      <c r="T90" s="40"/>
+      <c r="U90" s="40"/>
+      <c r="V90" s="40"/>
       <c r="W90" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="X90" s="67"/>
       <c r="Y90" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z90" s="67"/>
       <c r="AA90" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AB90" s="105"/>
       <c r="AC90" s="1"/>
@@ -5147,20 +5152,20 @@
       <c r="K91" s="72"/>
       <c r="L91" s="72"/>
       <c r="M91" s="75"/>
-      <c r="N91" s="29"/>
-      <c r="O91" s="29"/>
-      <c r="P91" s="29"/>
-      <c r="Q91" s="29"/>
-      <c r="R91" s="29"/>
-      <c r="S91" s="29"/>
-      <c r="T91" s="29"/>
-      <c r="U91" s="29"/>
-      <c r="V91" s="29"/>
-      <c r="W91" s="29"/>
-      <c r="X91" s="29"/>
-      <c r="Y91" s="29"/>
-      <c r="Z91" s="29"/>
-      <c r="AA91" s="29"/>
+      <c r="N91" s="40"/>
+      <c r="O91" s="40"/>
+      <c r="P91" s="40"/>
+      <c r="Q91" s="40"/>
+      <c r="R91" s="40"/>
+      <c r="S91" s="40"/>
+      <c r="T91" s="40"/>
+      <c r="U91" s="40"/>
+      <c r="V91" s="40"/>
+      <c r="W91" s="40"/>
+      <c r="X91" s="40"/>
+      <c r="Y91" s="40"/>
+      <c r="Z91" s="40"/>
+      <c r="AA91" s="40"/>
       <c r="AB91" s="96"/>
       <c r="AC91" s="1"/>
       <c r="AD91" s="1"/>
@@ -5174,7 +5179,7 @@
       <c r="B92" s="7"/>
       <c r="C92" s="8"/>
       <c r="D92" s="116" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E92" s="116"/>
       <c r="F92" s="116"/>
@@ -5186,7 +5191,7 @@
       <c r="L92" s="79"/>
       <c r="M92" s="75"/>
       <c r="N92" s="121" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="O92" s="121"/>
       <c r="P92" s="121"/>
@@ -5250,7 +5255,7 @@
       <c r="B94" s="7"/>
       <c r="C94" s="8"/>
       <c r="D94" s="119" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E94" s="119"/>
       <c r="F94" s="119"/>
@@ -5262,7 +5267,7 @@
       <c r="L94" s="79"/>
       <c r="M94" s="75"/>
       <c r="N94" s="121" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="O94" s="121"/>
       <c r="P94" s="121"/>
@@ -5326,7 +5331,7 @@
       <c r="B96" s="7"/>
       <c r="C96" s="8"/>
       <c r="D96" s="123" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E96" s="123"/>
       <c r="F96" s="123"/>
@@ -5338,7 +5343,7 @@
       <c r="L96" s="79"/>
       <c r="M96" s="75"/>
       <c r="N96" s="125" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="O96" s="125"/>
       <c r="P96" s="125"/>
@@ -5402,7 +5407,7 @@
       <c r="B98" s="7"/>
       <c r="C98" s="8"/>
       <c r="D98" s="119" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E98" s="119"/>
       <c r="F98" s="119"/>
@@ -5414,7 +5419,7 @@
       <c r="L98" s="79"/>
       <c r="M98" s="75"/>
       <c r="N98" s="121" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O98" s="121"/>
       <c r="P98" s="121"/>
@@ -5478,7 +5483,7 @@
       <c r="B100" s="7"/>
       <c r="C100" s="8"/>
       <c r="D100" s="116" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E100" s="116"/>
       <c r="F100" s="116"/>
@@ -5490,7 +5495,7 @@
       <c r="L100" s="79"/>
       <c r="M100" s="75"/>
       <c r="N100" s="125" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="O100" s="125"/>
       <c r="P100" s="125"/>
@@ -5553,20 +5558,20 @@
       <c r="A102" s="6"/>
       <c r="B102" s="7"/>
       <c r="C102" s="8"/>
-      <c r="D102" s="27" t="s">
-        <v>100</v>
+      <c r="D102" s="25" t="s">
+        <v>101</v>
       </c>
-      <c r="E102" s="27"/>
-      <c r="F102" s="27"/>
-      <c r="G102" s="27"/>
-      <c r="H102" s="27"/>
-      <c r="I102" s="27"/>
-      <c r="J102" s="27"/>
-      <c r="K102" s="27"/>
-      <c r="L102" s="27"/>
-      <c r="M102" s="29"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
+      <c r="G102" s="25"/>
+      <c r="H102" s="25"/>
+      <c r="I102" s="25"/>
+      <c r="J102" s="25"/>
+      <c r="K102" s="25"/>
+      <c r="L102" s="25"/>
+      <c r="M102" s="40"/>
       <c r="N102" s="121" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="O102" s="121"/>
       <c r="P102" s="121"/>
@@ -5593,16 +5598,16 @@
       <c r="A103" s="6"/>
       <c r="B103" s="7"/>
       <c r="C103" s="8"/>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
-      <c r="G103" s="29"/>
-      <c r="H103" s="29"/>
-      <c r="I103" s="29"/>
-      <c r="J103" s="29"/>
-      <c r="K103" s="29"/>
-      <c r="L103" s="29"/>
-      <c r="M103" s="29"/>
+      <c r="D103" s="40"/>
+      <c r="E103" s="40"/>
+      <c r="F103" s="40"/>
+      <c r="G103" s="40"/>
+      <c r="H103" s="40"/>
+      <c r="I103" s="40"/>
+      <c r="J103" s="40"/>
+      <c r="K103" s="40"/>
+      <c r="L103" s="40"/>
+      <c r="M103" s="40"/>
       <c r="N103" s="130"/>
       <c r="O103" s="130"/>
       <c r="P103" s="130"/>
@@ -5630,25 +5635,25 @@
       <c r="B104" s="7"/>
       <c r="C104" s="8"/>
       <c r="D104" s="65" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E104" s="65"/>
       <c r="F104" s="66"/>
       <c r="G104" s="66"/>
       <c r="H104" s="67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="I104" s="67"/>
       <c r="J104" s="67" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="K104" s="67"/>
       <c r="L104" s="67" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
-      <c r="M104" s="29"/>
+      <c r="M104" s="40"/>
       <c r="N104" s="116" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="O104" s="68"/>
       <c r="P104" s="68"/>
@@ -5678,7 +5683,7 @@
       <c r="J105" s="66"/>
       <c r="K105" s="66"/>
       <c r="L105" s="66"/>
-      <c r="M105" s="29"/>
+      <c r="M105" s="40"/>
       <c r="N105" s="133"/>
       <c r="O105" s="134"/>
       <c r="P105" s="134"/>
@@ -5700,7 +5705,7 @@
       <c r="B106" s="7"/>
       <c r="C106" s="8"/>
       <c r="D106" s="85" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E106" s="85"/>
       <c r="F106" s="125"/>
@@ -5712,7 +5717,7 @@
       <c r="L106" s="79"/>
       <c r="M106" s="75"/>
       <c r="N106" s="133" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="O106" s="134"/>
       <c r="P106" s="134"/>
@@ -5770,11 +5775,11 @@
       <c r="B108" s="7"/>
       <c r="C108" s="8"/>
       <c r="D108" s="76" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E108" s="76"/>
-      <c r="F108" s="34"/>
-      <c r="G108" s="34"/>
+      <c r="F108" s="33"/>
+      <c r="G108" s="33"/>
       <c r="H108" s="136"/>
       <c r="I108" s="137"/>
       <c r="J108" s="73"/>
@@ -5818,7 +5823,7 @@
       <c r="L109" s="137"/>
       <c r="M109" s="75"/>
       <c r="N109" s="141" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O109" s="141"/>
       <c r="P109" s="141"/>
@@ -5846,7 +5851,7 @@
       <c r="B110" s="7"/>
       <c r="C110" s="8"/>
       <c r="D110" s="85" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E110" s="85"/>
       <c r="F110" s="125"/>
@@ -5920,11 +5925,11 @@
       <c r="B112" s="7"/>
       <c r="C112" s="8"/>
       <c r="D112" s="76" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
-      <c r="E112" s="34"/>
-      <c r="F112" s="34"/>
-      <c r="G112" s="34"/>
+      <c r="E112" s="33"/>
+      <c r="F112" s="33"/>
+      <c r="G112" s="33"/>
       <c r="H112" s="136"/>
       <c r="I112" s="137"/>
       <c r="J112" s="73"/>
@@ -5932,7 +5937,7 @@
       <c r="L112" s="79"/>
       <c r="M112" s="75"/>
       <c r="N112" s="142" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="O112" s="142"/>
       <c r="P112" s="142"/>
@@ -5940,7 +5945,7 @@
       <c r="R112" s="142"/>
       <c r="S112" s="142"/>
       <c r="T112" s="143" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="U112" s="143"/>
       <c r="V112" s="143"/>
@@ -5998,7 +6003,7 @@
       <c r="B114" s="7"/>
       <c r="C114" s="8"/>
       <c r="D114" s="125" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E114" s="125"/>
       <c r="F114" s="125"/>
@@ -6010,7 +6015,7 @@
       <c r="L114" s="79"/>
       <c r="M114" s="75"/>
       <c r="N114" s="125" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O114" s="125"/>
       <c r="P114" s="125"/>
@@ -6018,7 +6023,7 @@
       <c r="R114" s="125"/>
       <c r="S114" s="125"/>
       <c r="T114" s="145" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="U114" s="145"/>
       <c r="V114" s="145"/>
@@ -6075,10 +6080,10 @@
       <c r="A116" s="6"/>
       <c r="B116" s="7"/>
       <c r="C116" s="8"/>
-      <c r="D116" s="34"/>
-      <c r="E116" s="34"/>
-      <c r="F116" s="34"/>
-      <c r="G116" s="34"/>
+      <c r="D116" s="33"/>
+      <c r="E116" s="33"/>
+      <c r="F116" s="33"/>
+      <c r="G116" s="33"/>
       <c r="H116" s="136"/>
       <c r="I116" s="137"/>
       <c r="J116" s="73"/>
@@ -6086,7 +6091,7 @@
       <c r="L116" s="79"/>
       <c r="M116" s="75"/>
       <c r="N116" s="142" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="O116" s="142"/>
       <c r="P116" s="142"/>
@@ -6094,7 +6099,7 @@
       <c r="R116" s="142"/>
       <c r="S116" s="142"/>
       <c r="T116" s="143" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="U116" s="143"/>
       <c r="V116" s="143"/>
@@ -29737,7 +29742,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="82">
     <mergeCell ref="C3:AB3"/>
     <mergeCell ref="A4:A120"/>
     <mergeCell ref="D4:D6"/>
@@ -29747,9 +29752,10 @@
     <mergeCell ref="E8:M8"/>
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="Q8:AA8"/>
-    <mergeCell ref="E10:M10"/>
-    <mergeCell ref="P10:AA10"/>
-    <mergeCell ref="D11:AA11"/>
+    <mergeCell ref="D10:AA10"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="P11:AA11"/>
+    <mergeCell ref="D12:AA12"/>
     <mergeCell ref="E13:AA13"/>
     <mergeCell ref="E14:M14"/>
     <mergeCell ref="N14:T14"/>
@@ -29840,7 +29846,7 @@
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="1" sqref="W38:AA48 D10"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10:AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29950,30 +29956,30 @@
     <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
       <c r="B3" s="7"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
+      <c r="D3" s="40"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
+      <c r="K3" s="40"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="40"/>
+      <c r="N3" s="40"/>
+      <c r="O3" s="40"/>
+      <c r="P3" s="40"/>
+      <c r="Q3" s="40"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="40"/>
+      <c r="T3" s="40"/>
+      <c r="U3" s="40"/>
+      <c r="V3" s="40"/>
+      <c r="W3" s="40"/>
+      <c r="X3" s="40"/>
+      <c r="Y3" s="40"/>
+      <c r="Z3" s="40"/>
+      <c r="AA3" s="40"/>
       <c r="AB3" s="128"/>
     </row>
     <row r="4" customFormat="false" ht="9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30011,7 +30017,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
       <c r="D5" s="157" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="E5" s="157"/>
       <c r="F5" s="157"/>
@@ -30263,7 +30269,7 @@
       <c r="N13" s="172"/>
       <c r="O13" s="172"/>
       <c r="P13" s="173" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="Q13" s="173"/>
       <c r="R13" s="173"/>
@@ -30293,7 +30299,7 @@
       <c r="N14" s="172"/>
       <c r="O14" s="172"/>
       <c r="P14" s="174" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="Q14" s="174"/>
       <c r="R14" s="174"/>
@@ -30301,7 +30307,7 @@
       <c r="T14" s="174"/>
       <c r="U14" s="175"/>
       <c r="V14" s="176" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="W14" s="176"/>
       <c r="X14" s="176"/>
@@ -30325,7 +30331,7 @@
       <c r="N15" s="172"/>
       <c r="O15" s="172"/>
       <c r="P15" s="174" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="Q15" s="174"/>
       <c r="R15" s="174"/>
@@ -30333,7 +30339,7 @@
       <c r="T15" s="174"/>
       <c r="U15" s="175"/>
       <c r="V15" s="176" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="W15" s="176"/>
       <c r="X15" s="176"/>
@@ -30357,7 +30363,7 @@
       <c r="N16" s="172"/>
       <c r="O16" s="172"/>
       <c r="P16" s="174" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Q16" s="174"/>
       <c r="R16" s="174"/>
@@ -30365,7 +30371,7 @@
       <c r="T16" s="174"/>
       <c r="U16" s="175"/>
       <c r="V16" s="176" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="W16" s="176"/>
       <c r="X16" s="176"/>
@@ -30501,7 +30507,7 @@
     <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="8"/>
       <c r="D21" s="183" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E21" s="183"/>
       <c r="F21" s="183"/>
@@ -30559,7 +30565,7 @@
     <row r="23" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="8"/>
       <c r="D23" s="183" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E23" s="172"/>
       <c r="F23" s="172"/>
@@ -30729,7 +30735,7 @@
     <row r="29" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="8"/>
       <c r="D29" s="184" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E29" s="184"/>
       <c r="F29" s="184"/>
@@ -30983,7 +30989,7 @@
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="8"/>
       <c r="D38" s="189" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E38" s="189"/>
       <c r="F38" s="189"/>
@@ -30995,7 +31001,7 @@
       <c r="L38" s="189"/>
       <c r="M38" s="190"/>
       <c r="N38" s="189" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="O38" s="189"/>
       <c r="P38" s="189"/>
@@ -31015,7 +31021,7 @@
     <row r="39" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="8"/>
       <c r="D39" s="191" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="E39" s="191"/>
       <c r="F39" s="191"/>
@@ -31027,7 +31033,7 @@
       <c r="L39" s="191"/>
       <c r="M39" s="192"/>
       <c r="N39" s="193" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O39" s="193"/>
       <c r="P39" s="193"/>

</xml_diff>

<commit_message>
media lista de cotejo
</commit_message>
<xml_diff>
--- a/public/assets/templates/camioneta.xlsx
+++ b/public/assets/templates/camioneta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAMIONETA" sheetId="1" state="visible" r:id="rId2"/>
@@ -73,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="132">
   <si>
     <t xml:space="preserve">INSPECCION MECANICA VEHICULAR PREVENTIVA</t>
   </si>
@@ -444,10 +444,19 @@
     <t xml:space="preserve">Llanta T LDI :</t>
   </si>
   <si>
-    <t xml:space="preserve">APROBADO : SI ________NO _________</t>
+    <t xml:space="preserve">SI</t>
   </si>
   <si>
-    <t xml:space="preserve">NOTA : </t>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">APROBADO:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">___</t>
+  </si>
+  <si>
+    <t xml:space="preserve">____</t>
   </si>
   <si>
     <t xml:space="preserve">OBSERVACIONES / COMENTARIOS / COMPROMISOS</t>
@@ -474,7 +483,7 @@
     <numFmt numFmtId="165" formatCode="[$-F800]dddd&quot;, &quot;mmmm\ dd&quot;, &quot;yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="40">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -738,6 +747,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="14"/>
+      <color rgb="FF111111"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
@@ -762,7 +785,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00275A"/>
-        <bgColor rgb="FF003300"/>
+        <bgColor rgb="FF111111"/>
       </patternFill>
     </fill>
     <fill>
@@ -952,7 +975,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="202">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1681,8 +1704,16 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1709,7 +1740,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="37" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="39" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1817,7 +1848,7 @@
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF00275A"/>
       <rgbColor rgb="FF00B050"/>
-      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF111111"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
@@ -1877,8 +1908,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H39" activeCellId="0" sqref="H39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H39" activeCellId="1" sqref="D24:AA25 H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29824,8 +29855,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24:AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -29837,7 +29868,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="4.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="3.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="4.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="5.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="1.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="5.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="1.5"/>
@@ -30459,9 +30490,13 @@
       <c r="C20" s="8"/>
       <c r="D20" s="171"/>
       <c r="E20" s="171"/>
-      <c r="F20" s="171"/>
+      <c r="F20" s="171" t="s">
+        <v>122</v>
+      </c>
       <c r="G20" s="171"/>
-      <c r="H20" s="171"/>
+      <c r="H20" s="182" t="s">
+        <v>123</v>
+      </c>
       <c r="I20" s="171"/>
       <c r="J20" s="171"/>
       <c r="K20" s="171"/>
@@ -30485,14 +30520,18 @@
     </row>
     <row r="21" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C21" s="8"/>
-      <c r="D21" s="182" t="s">
-        <v>122</v>
+      <c r="D21" s="183" t="s">
+        <v>124</v>
       </c>
-      <c r="E21" s="182"/>
-      <c r="F21" s="182"/>
-      <c r="G21" s="182"/>
-      <c r="H21" s="182"/>
-      <c r="I21" s="182"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="158" t="s">
+        <v>125</v>
+      </c>
+      <c r="G21" s="0"/>
+      <c r="H21" s="158" t="s">
+        <v>126</v>
+      </c>
+      <c r="I21" s="183"/>
       <c r="J21" s="171"/>
       <c r="K21" s="171"/>
       <c r="L21" s="171"/>
@@ -30543,9 +30582,7 @@
     </row>
     <row r="23" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C23" s="8"/>
-      <c r="D23" s="182" t="s">
-        <v>123</v>
-      </c>
+      <c r="D23" s="183"/>
       <c r="E23" s="171"/>
       <c r="F23" s="171"/>
       <c r="G23" s="171"/>
@@ -30573,7 +30610,7 @@
     </row>
     <row r="24" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C24" s="8"/>
-      <c r="D24" s="171"/>
+      <c r="D24" s="184"/>
       <c r="E24" s="171"/>
       <c r="F24" s="171"/>
       <c r="G24" s="171"/>
@@ -30713,32 +30750,32 @@
     </row>
     <row r="29" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C29" s="8"/>
-      <c r="D29" s="183" t="s">
-        <v>124</v>
+      <c r="D29" s="185" t="s">
+        <v>127</v>
       </c>
-      <c r="E29" s="183"/>
-      <c r="F29" s="183"/>
-      <c r="G29" s="183"/>
-      <c r="H29" s="183"/>
-      <c r="I29" s="183"/>
-      <c r="J29" s="183"/>
-      <c r="K29" s="183"/>
-      <c r="L29" s="183"/>
-      <c r="M29" s="183"/>
-      <c r="N29" s="183"/>
-      <c r="O29" s="183"/>
-      <c r="P29" s="183"/>
-      <c r="Q29" s="183"/>
-      <c r="R29" s="183"/>
-      <c r="S29" s="183"/>
-      <c r="T29" s="183"/>
-      <c r="U29" s="183"/>
-      <c r="V29" s="183"/>
-      <c r="W29" s="183"/>
-      <c r="X29" s="183"/>
-      <c r="Y29" s="183"/>
-      <c r="Z29" s="183"/>
-      <c r="AA29" s="183"/>
+      <c r="E29" s="185"/>
+      <c r="F29" s="185"/>
+      <c r="G29" s="185"/>
+      <c r="H29" s="185"/>
+      <c r="I29" s="185"/>
+      <c r="J29" s="185"/>
+      <c r="K29" s="185"/>
+      <c r="L29" s="185"/>
+      <c r="M29" s="185"/>
+      <c r="N29" s="185"/>
+      <c r="O29" s="185"/>
+      <c r="P29" s="185"/>
+      <c r="Q29" s="185"/>
+      <c r="R29" s="185"/>
+      <c r="S29" s="185"/>
+      <c r="T29" s="185"/>
+      <c r="U29" s="185"/>
+      <c r="V29" s="185"/>
+      <c r="W29" s="185"/>
+      <c r="X29" s="185"/>
+      <c r="Y29" s="185"/>
+      <c r="Z29" s="185"/>
+      <c r="AA29" s="185"/>
       <c r="AB29" s="157"/>
     </row>
     <row r="30" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -30939,207 +30976,207 @@
     </row>
     <row r="37" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="8"/>
-      <c r="D37" s="184"/>
-      <c r="E37" s="184"/>
-      <c r="F37" s="184"/>
-      <c r="G37" s="184"/>
-      <c r="H37" s="184"/>
-      <c r="I37" s="184"/>
-      <c r="J37" s="184"/>
-      <c r="K37" s="184"/>
-      <c r="L37" s="184"/>
-      <c r="M37" s="185"/>
-      <c r="N37" s="186"/>
-      <c r="O37" s="186"/>
-      <c r="P37" s="186"/>
-      <c r="Q37" s="186"/>
-      <c r="R37" s="186"/>
-      <c r="S37" s="186"/>
-      <c r="T37" s="186"/>
-      <c r="U37" s="186"/>
-      <c r="V37" s="186"/>
-      <c r="W37" s="186"/>
-      <c r="X37" s="186"/>
-      <c r="Y37" s="186"/>
-      <c r="Z37" s="186"/>
-      <c r="AA37" s="186"/>
-      <c r="AB37" s="187"/>
+      <c r="D37" s="186"/>
+      <c r="E37" s="186"/>
+      <c r="F37" s="186"/>
+      <c r="G37" s="186"/>
+      <c r="H37" s="186"/>
+      <c r="I37" s="186"/>
+      <c r="J37" s="186"/>
+      <c r="K37" s="186"/>
+      <c r="L37" s="186"/>
+      <c r="M37" s="187"/>
+      <c r="N37" s="188"/>
+      <c r="O37" s="188"/>
+      <c r="P37" s="188"/>
+      <c r="Q37" s="188"/>
+      <c r="R37" s="188"/>
+      <c r="S37" s="188"/>
+      <c r="T37" s="188"/>
+      <c r="U37" s="188"/>
+      <c r="V37" s="188"/>
+      <c r="W37" s="188"/>
+      <c r="X37" s="188"/>
+      <c r="Y37" s="188"/>
+      <c r="Z37" s="188"/>
+      <c r="AA37" s="188"/>
+      <c r="AB37" s="189"/>
     </row>
     <row r="38" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C38" s="8"/>
-      <c r="D38" s="188" t="s">
-        <v>125</v>
+      <c r="D38" s="190" t="s">
+        <v>128</v>
       </c>
-      <c r="E38" s="188"/>
-      <c r="F38" s="188"/>
-      <c r="G38" s="188"/>
-      <c r="H38" s="188"/>
-      <c r="I38" s="188"/>
-      <c r="J38" s="188"/>
-      <c r="K38" s="188"/>
-      <c r="L38" s="188"/>
-      <c r="M38" s="189"/>
-      <c r="N38" s="188" t="s">
-        <v>126</v>
+      <c r="E38" s="190"/>
+      <c r="F38" s="190"/>
+      <c r="G38" s="190"/>
+      <c r="H38" s="190"/>
+      <c r="I38" s="190"/>
+      <c r="J38" s="190"/>
+      <c r="K38" s="190"/>
+      <c r="L38" s="190"/>
+      <c r="M38" s="191"/>
+      <c r="N38" s="190" t="s">
+        <v>129</v>
       </c>
-      <c r="O38" s="188"/>
-      <c r="P38" s="188"/>
-      <c r="Q38" s="188"/>
-      <c r="R38" s="188"/>
-      <c r="S38" s="188"/>
-      <c r="T38" s="188"/>
-      <c r="U38" s="188"/>
-      <c r="V38" s="188"/>
-      <c r="W38" s="188"/>
-      <c r="X38" s="188"/>
-      <c r="Y38" s="188"/>
-      <c r="Z38" s="188"/>
-      <c r="AA38" s="188"/>
+      <c r="O38" s="190"/>
+      <c r="P38" s="190"/>
+      <c r="Q38" s="190"/>
+      <c r="R38" s="190"/>
+      <c r="S38" s="190"/>
+      <c r="T38" s="190"/>
+      <c r="U38" s="190"/>
+      <c r="V38" s="190"/>
+      <c r="W38" s="190"/>
+      <c r="X38" s="190"/>
+      <c r="Y38" s="190"/>
+      <c r="Z38" s="190"/>
+      <c r="AA38" s="190"/>
       <c r="AB38" s="160"/>
     </row>
     <row r="39" customFormat="false" ht="87" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C39" s="8"/>
-      <c r="D39" s="190" t="s">
-        <v>127</v>
+      <c r="D39" s="192" t="s">
+        <v>130</v>
       </c>
-      <c r="E39" s="190"/>
-      <c r="F39" s="190"/>
-      <c r="G39" s="190"/>
-      <c r="H39" s="190"/>
-      <c r="I39" s="190"/>
-      <c r="J39" s="190"/>
-      <c r="K39" s="190"/>
-      <c r="L39" s="190"/>
-      <c r="M39" s="191"/>
-      <c r="N39" s="192" t="s">
-        <v>128</v>
+      <c r="E39" s="192"/>
+      <c r="F39" s="192"/>
+      <c r="G39" s="192"/>
+      <c r="H39" s="192"/>
+      <c r="I39" s="192"/>
+      <c r="J39" s="192"/>
+      <c r="K39" s="192"/>
+      <c r="L39" s="192"/>
+      <c r="M39" s="193"/>
+      <c r="N39" s="194" t="s">
+        <v>131</v>
       </c>
-      <c r="O39" s="192"/>
-      <c r="P39" s="192"/>
-      <c r="Q39" s="192"/>
-      <c r="R39" s="192"/>
-      <c r="S39" s="192"/>
-      <c r="T39" s="192"/>
-      <c r="U39" s="192"/>
-      <c r="V39" s="192"/>
-      <c r="W39" s="192"/>
-      <c r="X39" s="192"/>
-      <c r="Y39" s="192"/>
-      <c r="Z39" s="192"/>
-      <c r="AA39" s="192"/>
+      <c r="O39" s="194"/>
+      <c r="P39" s="194"/>
+      <c r="Q39" s="194"/>
+      <c r="R39" s="194"/>
+      <c r="S39" s="194"/>
+      <c r="T39" s="194"/>
+      <c r="U39" s="194"/>
+      <c r="V39" s="194"/>
+      <c r="W39" s="194"/>
+      <c r="X39" s="194"/>
+      <c r="Y39" s="194"/>
+      <c r="Z39" s="194"/>
+      <c r="AA39" s="194"/>
       <c r="AB39" s="161"/>
     </row>
     <row r="40" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C40" s="8"/>
-      <c r="D40" s="191"/>
-      <c r="E40" s="191"/>
-      <c r="F40" s="191"/>
-      <c r="G40" s="191"/>
-      <c r="H40" s="191"/>
-      <c r="I40" s="191"/>
-      <c r="J40" s="191"/>
-      <c r="K40" s="191"/>
-      <c r="L40" s="191"/>
-      <c r="M40" s="191"/>
-      <c r="N40" s="193"/>
-      <c r="O40" s="193"/>
-      <c r="P40" s="193"/>
-      <c r="Q40" s="193"/>
-      <c r="R40" s="193"/>
-      <c r="S40" s="193"/>
-      <c r="T40" s="193"/>
-      <c r="U40" s="193"/>
-      <c r="V40" s="193"/>
-      <c r="W40" s="193"/>
-      <c r="X40" s="193"/>
-      <c r="Y40" s="193"/>
-      <c r="Z40" s="193"/>
-      <c r="AA40" s="193"/>
+      <c r="D40" s="193"/>
+      <c r="E40" s="193"/>
+      <c r="F40" s="193"/>
+      <c r="G40" s="193"/>
+      <c r="H40" s="193"/>
+      <c r="I40" s="193"/>
+      <c r="J40" s="193"/>
+      <c r="K40" s="193"/>
+      <c r="L40" s="193"/>
+      <c r="M40" s="193"/>
+      <c r="N40" s="195"/>
+      <c r="O40" s="195"/>
+      <c r="P40" s="195"/>
+      <c r="Q40" s="195"/>
+      <c r="R40" s="195"/>
+      <c r="S40" s="195"/>
+      <c r="T40" s="195"/>
+      <c r="U40" s="195"/>
+      <c r="V40" s="195"/>
+      <c r="W40" s="195"/>
+      <c r="X40" s="195"/>
+      <c r="Y40" s="195"/>
+      <c r="Z40" s="195"/>
+      <c r="AA40" s="195"/>
       <c r="AB40" s="162"/>
     </row>
     <row r="41" customFormat="false" ht="45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C41" s="8"/>
-      <c r="D41" s="191"/>
-      <c r="E41" s="191"/>
-      <c r="F41" s="191"/>
-      <c r="G41" s="191"/>
-      <c r="H41" s="191"/>
-      <c r="I41" s="191"/>
-      <c r="J41" s="191"/>
-      <c r="K41" s="191"/>
-      <c r="L41" s="191"/>
-      <c r="M41" s="191"/>
-      <c r="N41" s="193"/>
-      <c r="O41" s="193"/>
-      <c r="P41" s="193"/>
-      <c r="Q41" s="193"/>
-      <c r="R41" s="193"/>
-      <c r="S41" s="193"/>
-      <c r="T41" s="193"/>
-      <c r="U41" s="193"/>
-      <c r="V41" s="193"/>
-      <c r="W41" s="193"/>
-      <c r="X41" s="193"/>
-      <c r="Y41" s="193"/>
-      <c r="Z41" s="193"/>
-      <c r="AA41" s="193"/>
+      <c r="D41" s="193"/>
+      <c r="E41" s="193"/>
+      <c r="F41" s="193"/>
+      <c r="G41" s="193"/>
+      <c r="H41" s="193"/>
+      <c r="I41" s="193"/>
+      <c r="J41" s="193"/>
+      <c r="K41" s="193"/>
+      <c r="L41" s="193"/>
+      <c r="M41" s="193"/>
+      <c r="N41" s="195"/>
+      <c r="O41" s="195"/>
+      <c r="P41" s="195"/>
+      <c r="Q41" s="195"/>
+      <c r="R41" s="195"/>
+      <c r="S41" s="195"/>
+      <c r="T41" s="195"/>
+      <c r="U41" s="195"/>
+      <c r="V41" s="195"/>
+      <c r="W41" s="195"/>
+      <c r="X41" s="195"/>
+      <c r="Y41" s="195"/>
+      <c r="Z41" s="195"/>
+      <c r="AA41" s="195"/>
       <c r="AB41" s="162"/>
     </row>
     <row r="42" customFormat="false" ht="28.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C42" s="8"/>
-      <c r="D42" s="194"/>
-      <c r="E42" s="194"/>
-      <c r="F42" s="194"/>
-      <c r="G42" s="194"/>
-      <c r="H42" s="194"/>
-      <c r="I42" s="194"/>
-      <c r="J42" s="194"/>
-      <c r="K42" s="194"/>
-      <c r="L42" s="194"/>
+      <c r="D42" s="196"/>
+      <c r="E42" s="196"/>
+      <c r="F42" s="196"/>
+      <c r="G42" s="196"/>
+      <c r="H42" s="196"/>
+      <c r="I42" s="196"/>
+      <c r="J42" s="196"/>
+      <c r="K42" s="196"/>
+      <c r="L42" s="196"/>
       <c r="M42" s="164"/>
-      <c r="N42" s="195"/>
-      <c r="O42" s="195"/>
-      <c r="P42" s="195"/>
-      <c r="Q42" s="195"/>
-      <c r="R42" s="195"/>
-      <c r="S42" s="195"/>
-      <c r="T42" s="195"/>
-      <c r="U42" s="195"/>
-      <c r="V42" s="195"/>
-      <c r="W42" s="195"/>
-      <c r="X42" s="195"/>
-      <c r="Y42" s="195"/>
-      <c r="Z42" s="195"/>
-      <c r="AA42" s="195"/>
-      <c r="AB42" s="196"/>
+      <c r="N42" s="197"/>
+      <c r="O42" s="197"/>
+      <c r="P42" s="197"/>
+      <c r="Q42" s="197"/>
+      <c r="R42" s="197"/>
+      <c r="S42" s="197"/>
+      <c r="T42" s="197"/>
+      <c r="U42" s="197"/>
+      <c r="V42" s="197"/>
+      <c r="W42" s="197"/>
+      <c r="X42" s="197"/>
+      <c r="Y42" s="197"/>
+      <c r="Z42" s="197"/>
+      <c r="AA42" s="197"/>
+      <c r="AB42" s="198"/>
     </row>
     <row r="43" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C43" s="146"/>
-      <c r="D43" s="197"/>
-      <c r="E43" s="197"/>
-      <c r="F43" s="197"/>
-      <c r="G43" s="197"/>
-      <c r="H43" s="197"/>
-      <c r="I43" s="197"/>
-      <c r="J43" s="197"/>
-      <c r="K43" s="197"/>
-      <c r="L43" s="197"/>
-      <c r="M43" s="198"/>
-      <c r="N43" s="197"/>
-      <c r="O43" s="197"/>
-      <c r="P43" s="197"/>
-      <c r="Q43" s="197"/>
-      <c r="R43" s="197"/>
-      <c r="S43" s="197"/>
-      <c r="T43" s="197"/>
-      <c r="U43" s="197"/>
-      <c r="V43" s="197"/>
-      <c r="W43" s="197"/>
-      <c r="X43" s="197"/>
-      <c r="Y43" s="197"/>
-      <c r="Z43" s="197"/>
-      <c r="AA43" s="197"/>
-      <c r="AB43" s="199"/>
+      <c r="D43" s="199"/>
+      <c r="E43" s="199"/>
+      <c r="F43" s="199"/>
+      <c r="G43" s="199"/>
+      <c r="H43" s="199"/>
+      <c r="I43" s="199"/>
+      <c r="J43" s="199"/>
+      <c r="K43" s="199"/>
+      <c r="L43" s="199"/>
+      <c r="M43" s="200"/>
+      <c r="N43" s="199"/>
+      <c r="O43" s="199"/>
+      <c r="P43" s="199"/>
+      <c r="Q43" s="199"/>
+      <c r="R43" s="199"/>
+      <c r="S43" s="199"/>
+      <c r="T43" s="199"/>
+      <c r="U43" s="199"/>
+      <c r="V43" s="199"/>
+      <c r="W43" s="199"/>
+      <c r="X43" s="199"/>
+      <c r="Y43" s="199"/>
+      <c r="Z43" s="199"/>
+      <c r="AA43" s="199"/>
+      <c r="AB43" s="201"/>
     </row>
     <row r="44" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D44" s="152"/>
@@ -54809,7 +54846,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="20">
     <mergeCell ref="D5:AA5"/>
     <mergeCell ref="D6:L8"/>
     <mergeCell ref="N6:AA8"/>
@@ -54823,7 +54860,6 @@
     <mergeCell ref="V15:AA15"/>
     <mergeCell ref="P16:T16"/>
     <mergeCell ref="V16:AA16"/>
-    <mergeCell ref="D21:I21"/>
     <mergeCell ref="D29:AA29"/>
     <mergeCell ref="D30:AA35"/>
     <mergeCell ref="D38:L38"/>

</xml_diff>

<commit_message>
manejo de series con numero_certificado
</commit_message>
<xml_diff>
--- a/public/assets/templates/camioneta.xlsx
+++ b/public/assets/templates/camioneta.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="CAMIONETA" sheetId="1" state="visible" r:id="rId2"/>
@@ -87,19 +87,19 @@
     <t xml:space="preserve">C 0040</t>
   </si>
   <si>
-    <t xml:space="preserve">Fecha de inspección:</t>
+    <t xml:space="preserve">Fecha de inspección :</t>
   </si>
   <si>
-    <t xml:space="preserve">Vigencia Hasta:</t>
+    <t xml:space="preserve">Vigencia Hasta :</t>
   </si>
   <si>
     <t xml:space="preserve">DATOS DEL PROPIETARIO</t>
   </si>
   <si>
-    <t xml:space="preserve">Propietario</t>
+    <t xml:space="preserve">Propietario :</t>
   </si>
   <si>
-    <t xml:space="preserve">Identificación</t>
+    <t xml:space="preserve">Identificación :</t>
   </si>
   <si>
     <t xml:space="preserve">DATOS DEL CONDUCTOR</t>
@@ -108,16 +108,16 @@
     <t xml:space="preserve">Nombre Transportadora :</t>
   </si>
   <si>
-    <t xml:space="preserve">Nombres Conductor:</t>
+    <t xml:space="preserve">Nombres Conductor :</t>
   </si>
   <si>
-    <t xml:space="preserve">V / Licencia conduccion </t>
+    <t xml:space="preserve">V / Licencia conducción :</t>
   </si>
   <si>
     <t xml:space="preserve">No. Identificación :</t>
   </si>
   <si>
-    <t xml:space="preserve">Telefono :</t>
+    <t xml:space="preserve">Teléfono :</t>
   </si>
   <si>
     <t xml:space="preserve">DATOS DEL VEHÍCULO</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">Clase de vehículo :</t>
   </si>
   <si>
-    <t xml:space="preserve">SOAT:</t>
+    <t xml:space="preserve">SOAT :</t>
   </si>
   <si>
     <t xml:space="preserve">V:</t>
@@ -177,7 +177,7 @@
     <t xml:space="preserve">No Aplica </t>
   </si>
   <si>
-    <t xml:space="preserve">1. SISTEMA ELECTRICO </t>
+    <t xml:space="preserve">1. SISTEMA ELÉCTRICO </t>
   </si>
   <si>
     <t xml:space="preserve">5. SEGURIDAD ACTIVA</t>
@@ -234,7 +234,7 @@
     <t xml:space="preserve">Luz antineblina (exploradoras)</t>
   </si>
   <si>
-    <t xml:space="preserve">6. SISTEMA DE SEGRIDAD PASIVA </t>
+    <t xml:space="preserve">6. SISTEMA DE SEGURIDAD PASIVA </t>
   </si>
   <si>
     <t xml:space="preserve">Luz de placa</t>
@@ -252,10 +252,10 @@
     <t xml:space="preserve">Airbags (conductor - copiloto)</t>
   </si>
   <si>
-    <t xml:space="preserve">BATERÍA (bornes, nivel acido, fugas)</t>
+    <t xml:space="preserve">BATERÍA (bornes, nivel ácido, fugas)</t>
   </si>
   <si>
-    <t xml:space="preserve">Cadena de sujeción cardán</t>
+    <t xml:space="preserve">Cadena de sujeción cardan</t>
   </si>
   <si>
     <t xml:space="preserve">Aire acondicionado </t>
@@ -267,7 +267,7 @@
     <t xml:space="preserve">2. SISTEMA MOTOR </t>
   </si>
   <si>
-    <t xml:space="preserve">Apoyacabezas (todos las sillas)</t>
+    <t xml:space="preserve">Apoya-cabezas (todas las sillas)</t>
   </si>
   <si>
     <t xml:space="preserve">Barra antivuelco (anclada al chasis)</t>
@@ -279,7 +279,7 @@
     <t xml:space="preserve">Rejilla de protección vidrio trasero</t>
   </si>
   <si>
-    <t xml:space="preserve">Nivel  de aceite de Transmision</t>
+    <t xml:space="preserve">Nivel  de aceite de Transmisión</t>
   </si>
   <si>
     <t xml:space="preserve">7. KIT DE CARRETERA</t>
@@ -315,7 +315,7 @@
     <t xml:space="preserve">3.CARROCERIA / PARTE EXTERNA </t>
   </si>
   <si>
-    <t xml:space="preserve">Llanta de repuesto/ cruzeta</t>
+    <t xml:space="preserve">Llanta de repuesto/ cruceta</t>
   </si>
   <si>
     <t xml:space="preserve">Caja de Herramientas </t>
@@ -333,7 +333,7 @@
     <t xml:space="preserve">Gato con capacidad de subir el vehículo</t>
   </si>
   <si>
-    <t xml:space="preserve">Estado general vidirios de seguridad)</t>
+    <t xml:space="preserve">Estado general vidrios de seguridad)</t>
   </si>
   <si>
     <t xml:space="preserve">4.PARTE BAJA </t>
@@ -393,7 +393,7 @@
     <t xml:space="preserve">9. PROFUNDIDAD DE LABRADO DE LLANTAS </t>
   </si>
   <si>
-    <t xml:space="preserve">Vidrios Electricos </t>
+    <t xml:space="preserve">Vidrios Eléctricos </t>
   </si>
   <si>
     <t xml:space="preserve">Antideslizantes de pedales</t>
@@ -1712,7 +1712,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1870,9 +1870,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>2301480</xdr:colOff>
+      <xdr:colOff>2301120</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>480240</xdr:rowOff>
+      <xdr:rowOff>479880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1886,7 +1886,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="891000" y="399240"/>
-          <a:ext cx="2010600" cy="855000"/>
+          <a:ext cx="2010240" cy="854640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1908,8 +1908,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A136" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H39" activeCellId="1" sqref="D24:AA25 H39"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B74" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA66" activeCellId="0" sqref="AA66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2822,30 +2822,30 @@
       <c r="A29" s="6"/>
       <c r="B29" s="7"/>
       <c r="C29" s="8"/>
-      <c r="D29" s="0"/>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="I29" s="0"/>
-      <c r="J29" s="0"/>
-      <c r="K29" s="0"/>
-      <c r="L29" s="0"/>
-      <c r="M29" s="0"/>
-      <c r="N29" s="0"/>
-      <c r="O29" s="0"/>
-      <c r="P29" s="0"/>
-      <c r="Q29" s="0"/>
-      <c r="R29" s="0"/>
-      <c r="S29" s="0"/>
-      <c r="T29" s="0"/>
-      <c r="U29" s="0"/>
-      <c r="V29" s="0"/>
-      <c r="W29" s="0"/>
-      <c r="X29" s="0"/>
-      <c r="Y29" s="0"/>
-      <c r="Z29" s="0"/>
-      <c r="AA29" s="0"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="27"/>
+      <c r="N29" s="27"/>
+      <c r="O29" s="27"/>
+      <c r="P29" s="27"/>
+      <c r="Q29" s="27"/>
+      <c r="R29" s="27"/>
+      <c r="S29" s="27"/>
+      <c r="T29" s="27"/>
+      <c r="U29" s="27"/>
+      <c r="V29" s="27"/>
+      <c r="W29" s="27"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27"/>
+      <c r="AA29" s="27"/>
       <c r="AB29" s="13"/>
     </row>
     <row r="30" customFormat="false" ht="3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -29855,8 +29855,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A3" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24:AA25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.50390625" defaultRowHeight="21" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -30523,11 +30523,11 @@
       <c r="D21" s="183" t="s">
         <v>124</v>
       </c>
-      <c r="E21" s="0"/>
+      <c r="E21" s="27"/>
       <c r="F21" s="158" t="s">
         <v>125</v>
       </c>
-      <c r="G21" s="0"/>
+      <c r="G21" s="27"/>
       <c r="H21" s="158" t="s">
         <v>126</v>
       </c>

</xml_diff>